<commit_message>
CRM-3460 Add PO number on reference invoice id for buback PO reimbursement file
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Buyback-v1.xlsx
+++ b/application/controllers/excel-templates/Buyback-v1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD746F3-603D-4BAB-8760-AE20AB180ED7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C251A4BA-EA7B-4400-8099-B44D670E6132}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Blackmelon Advance Technology Co. Pvt. Ltd.</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>A-1/7, F/F A BLOCK, KRISHNA NAGAR, DELHI, 110051</t>
+  </si>
+  <si>
+    <t>Reference No: {meta:reference_invoice_id}</t>
   </si>
 </sst>
 </file>
@@ -899,7 +902,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1375,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1582,7 +1585,9 @@
       <c r="H9" s="49"/>
       <c r="I9" s="49"/>
       <c r="J9" s="64"/>
-      <c r="K9" s="67"/>
+      <c r="K9" s="67" t="s">
+        <v>35</v>
+      </c>
       <c r="L9" s="31"/>
       <c r="M9" s="31"/>
       <c r="N9" s="31"/>

</xml_diff>